<commit_message>
add Validation to Excel register sportsman , drop list coachId
</commit_message>
<xml_diff>
--- a/server/resources/files/רישום ספורטאים למערכת.xlsx
+++ b/server/resources/files/רישום ספורטאים למערכת.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>ת.ז ספורטאי</t>
   </si>
@@ -49,25 +49,13 @@
     <t>מועדנים</t>
   </si>
   <si>
-    <t>רחובות (קוד: 1)</t>
-  </si>
-  <si>
-    <t>לפיד ראשון (קוד: 2)</t>
-  </si>
-  <si>
-    <t>קרית גת (קוד: 3)</t>
-  </si>
-  <si>
-    <t>לוחמים בע"מ (קוד: 4)</t>
-  </si>
-  <si>
-    <t>הפועל בת ים (קוד: 5)</t>
-  </si>
-  <si>
     <t>מיטב חדרה (קוד: 6)</t>
   </si>
   <si>
-    <t>קונגפו-פנדה (קוד: 7)</t>
+    <t>מאמנים</t>
+  </si>
+  <si>
+    <t>שגיב מפגפקר (ת.ז: 305077914)</t>
   </si>
 </sst>
 </file>
@@ -131,7 +119,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:AA999"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="true" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomRight" state="frozen"/>
@@ -139,7 +127,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:27">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -176,48 +164,36 @@
       <c r="Z1" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="4:26">
+      <c r="AA1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="4:27">
       <c r="D2" s="4"/>
       <c r="Z2" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="4:26">
-      <c r="D3" s="4"/>
-      <c r="Z3" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="4:26">
-      <c r="D4" s="4"/>
-      <c r="Z4" s="3" t="s">
+      <c r="AA2" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="4:26">
+    <row r="3" spans="4:4">
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="4:4">
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="4:4">
       <c r="D5" s="4"/>
-      <c r="Z5" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="4:26">
+    </row>
+    <row r="6" spans="4:4">
       <c r="D6" s="4"/>
-      <c r="Z6" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="4:26">
+    </row>
+    <row r="7" spans="4:4">
       <c r="D7" s="4"/>
-      <c r="Z7" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="4:26">
+    </row>
+    <row r="8" spans="4:4">
       <c r="D8" s="4"/>
-      <c r="Z8" s="3" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="9" spans="4:4">
       <c r="D9" s="4"/>
@@ -3193,7 +3169,10 @@
       <c r="D999" s="4"/>
     </row>
   </sheetData>
-  <dataValidations count="7">
+  <dataValidations count="8">
+    <dataValidation type="list" allowBlank="0" showInputMessage="1" showErrorMessage="1" error="Invalid choice was chosen" prompt="בחר מועדון" sqref="K2:K100">
+      <formula1>=sheet1!$AA$2:$AA$2</formula1>
+    </dataValidation>
     <dataValidation type="textLength" allowBlank="0" showInputMessage="1" showErrorMessage="1" error="ת.ז צריכה להכיל 9 ספרות" prompt="הכנס ת.ז ספורטאי" sqref="K2:K100">
       <formula1>9</formula1>
       <formula2>9</formula2>
@@ -3207,7 +3186,7 @@
       <formula2>10</formula2>
     </dataValidation>
     <dataValidation type="list" allowBlank="0" showInputMessage="1" showErrorMessage="1" error="Invalid choice was chosen" prompt="בחר מועדון" sqref="H2:H100">
-      <formula1>=sheet1!$Z$2:$Z$8</formula1>
+      <formula1>=sheet1!$Z$2:$Z$2</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="0" showInputMessage="1" showErrorMessage="1" error="Invalid choice was chosen" prompt="בחר מין" sqref="I2:I100">
       <formula1>"זכר,נקבה"</formula1>

</xml_diff>

<commit_message>
* add birthdate validate * change error message
</commit_message>
<xml_diff>
--- a/server/resources/files/רישום ספורטאים למערכת.xlsx
+++ b/server/resources/files/רישום ספורטאים למערכת.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>ת.ז ספורטאי</t>
   </si>
@@ -49,13 +49,49 @@
     <t>מועדנים</t>
   </si>
   <si>
+    <t>רחובות (קוד: 1)</t>
+  </si>
+  <si>
+    <t>לפיד ראשון (קוד: 2)</t>
+  </si>
+  <si>
+    <t>קרית גת (קוד: 3)</t>
+  </si>
+  <si>
+    <t>לוחמים בע"מ (קוד: 4)</t>
+  </si>
+  <si>
+    <t>הפועל בת ים (קוד: 5)</t>
+  </si>
+  <si>
     <t>מיטב חדרה (קוד: 6)</t>
+  </si>
+  <si>
+    <t>קונגפו-פנדה (קוד: 7)</t>
   </si>
   <si>
     <t>מאמנים</t>
   </si>
   <si>
+    <t>לנה גלקר (ת.ז: 322232424)</t>
+  </si>
+  <si>
+    <t>אלכסנדר פרנקל (ת.ז: 305077910)</t>
+  </si>
+  <si>
+    <t>בארוך סגל (ת.ז: 305077911)</t>
+  </si>
+  <si>
+    <t>מישל שחר (ת.ז: 305077912)</t>
+  </si>
+  <si>
+    <t>שושי שופר (ת.ז: 305077913)</t>
+  </si>
+  <si>
     <t>שגיב מפגפקר (ת.ז: 305077914)</t>
+  </si>
+  <si>
+    <t>אור אפרים (ת.ז: 305077915)</t>
   </si>
 </sst>
 </file>
@@ -165,7 +201,7 @@
         <v>11</v>
       </c>
       <c r="AA1" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="4:27">
@@ -174,26 +210,62 @@
         <v>12</v>
       </c>
       <c r="AA2" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="4:27">
+      <c r="D3" s="4"/>
+      <c r="Z3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="4:27">
+      <c r="D4" s="4"/>
+      <c r="Z4" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="4:4">
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="4:4">
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="4:4">
+      <c r="AA4" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="4:27">
       <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="4:4">
+      <c r="Z5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA5" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="4:27">
       <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="4:4">
+      <c r="Z6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA6" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="4:27">
       <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="4:4">
+      <c r="Z7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA7" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="4:27">
       <c r="D8" s="4"/>
+      <c r="Z8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA8" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="4:4">
       <c r="D9" s="4"/>
@@ -3171,7 +3243,7 @@
   </sheetData>
   <dataValidations count="8">
     <dataValidation type="list" allowBlank="0" showInputMessage="1" showErrorMessage="1" error="Invalid choice was chosen" prompt="בחר מועדון" sqref="K2:K100">
-      <formula1>=sheet1!$AA$2:$AA$2</formula1>
+      <formula1>=sheet1!$AA$2:$AA$8</formula1>
     </dataValidation>
     <dataValidation type="textLength" allowBlank="0" showInputMessage="1" showErrorMessage="1" error="ת.ז צריכה להכיל 9 ספרות" prompt="הכנס ת.ז ספורטאי" sqref="K2:K100">
       <formula1>9</formula1>
@@ -3186,7 +3258,7 @@
       <formula2>10</formula2>
     </dataValidation>
     <dataValidation type="list" allowBlank="0" showInputMessage="1" showErrorMessage="1" error="Invalid choice was chosen" prompt="בחר מועדון" sqref="H2:H100">
-      <formula1>=sheet1!$Z$2:$Z$2</formula1>
+      <formula1>=sheet1!$Z$2:$Z$8</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="0" showInputMessage="1" showErrorMessage="1" error="Invalid choice was chosen" prompt="בחר מין" sqref="I2:I100">
       <formula1>"זכר,נקבה"</formula1>

</xml_diff>

<commit_message>
*register to competition tmp**
</commit_message>
<xml_diff>
--- a/server/resources/files/רישום ספורטאים למערכת.xlsx
+++ b/server/resources/files/רישום ספורטאים למערכת.xlsx
@@ -3241,7 +3241,40 @@
       <c r="D999" s="4"/>
     </row>
   </sheetData>
-  <dataValidations count="8">
+  <dataValidations count="26">
+    <dataValidation type="custom" allowBlank="0" showErrorMessage="1" error="אינך יכול לשנות תא זה." sqref="A1">
+      <formula1>"A1"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="0" showErrorMessage="1" error="אינך יכול לשנות תא זה." sqref="B1">
+      <formula1>"B1"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="0" showErrorMessage="1" error="אינך יכול לשנות תא זה." sqref="C1">
+      <formula1>"C1"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="0" showErrorMessage="1" error="אינך יכול לשנות תא זה." sqref="D1">
+      <formula1>"D1"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="0" showErrorMessage="1" error="אינך יכול לשנות תא זה." sqref="E1">
+      <formula1>"E1"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="0" showErrorMessage="1" error="אינך יכול לשנות תא זה." sqref="F1">
+      <formula1>"F1"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="0" showErrorMessage="1" error="אינך יכול לשנות תא זה." sqref="G1">
+      <formula1>"G1"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="0" showErrorMessage="1" error="אינך יכול לשנות תא זה." sqref="H1">
+      <formula1>"H1"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="0" showErrorMessage="1" error="אינך יכול לשנות תא זה." sqref="I1">
+      <formula1>"I1"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="0" showErrorMessage="1" error="אינך יכול לשנות תא זה." sqref="J1">
+      <formula1>"J1"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="0" showErrorMessage="1" error="אינך יכול לשנות תא זה." sqref="K1">
+      <formula1>"K1"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="0" showInputMessage="1" showErrorMessage="1" error="Invalid choice was chosen" prompt="בחר מועדון" sqref="K2:K100">
       <formula1>=sheet1!$AA$2:$AA$8</formula1>
     </dataValidation>
@@ -3267,6 +3300,27 @@
       <formula1>"טאולו,סנדא"</formula1>
     </dataValidation>
     <dataValidation type="date" allowBlank="0" showInputMessage="1" showErrorMessage="1" error="פורמט תאריך צריך להיות dd/mm/yyyy" prompt="כתוב תאריך לידה בפורמט dd/mm/yyyy" sqref="F2:F100"/>
+    <dataValidation type="textLength" operator="equal" showErrorMessage="1" error="This cell is locked" sqref="L1:L100">
+      <formula1>""</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="equal" showErrorMessage="1" error="This cell is locked" sqref="M1:M100">
+      <formula1>""</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="equal" showErrorMessage="1" error="This cell is locked" sqref="N1:N100">
+      <formula1>""</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="equal" showErrorMessage="1" error="This cell is locked" sqref="O1:O100">
+      <formula1>""</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="equal" showErrorMessage="1" error="This cell is locked" sqref="P1:P100">
+      <formula1>""</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="equal" showErrorMessage="1" error="This cell is locked" sqref="Q1:Q100">
+      <formula1>""</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="equal" showErrorMessage="1" error="This cell is locked" sqref="R1:R100">
+      <formula1>""</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>